<commit_message>
Centrar titulo y formatear fecha en exportar a Excel
</commit_message>
<xml_diff>
--- a/tp_final/movimientos.xlsx
+++ b/tp_final/movimientos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Movimientos de cuenta bancaria</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>Saldo</t>
+  </si>
+  <si>
+    <t>07/01/2019</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
   </si>
 </sst>
 </file>
@@ -162,7 +168,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.609375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="12.70703125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -205,11 +211,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>43472.12744710648</v>
-      </c>
-      <c r="B7" t="n">
-        <v>7.0</v>
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
       </c>
       <c r="C7" t="n" s="9">
         <v>0.0</v>
@@ -222,11 +228,11 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>43472.12744759259</v>
-      </c>
-      <c r="B8" t="n">
-        <v>8.0</v>
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
       </c>
       <c r="C8" t="n" s="12">
         <v>2500.0</v>
@@ -239,6 +245,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>